<commit_message>
feat: planos de tdd abp & projeto aula
</commit_message>
<xml_diff>
--- a/5DSM - Agenda aulas ABP - 2025-2.xlsx
+++ b/5DSM - Agenda aulas ABP - 2025-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\5dsm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE172D5-F151-4FED-B9C1-F8011780BE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C646243A-E8FA-4522-9D9A-4B1DA802FF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{5A79BD2C-7FB4-4CDA-88C4-C274EF65DA92}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5A79BD2C-7FB4-4CDA-88C4-C274EF65DA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="2" r:id="rId1"/>
@@ -603,20 +603,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F909374-D5BD-4605-958A-DE380CAC4265}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -626,7 +626,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
@@ -636,7 +636,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -648,7 +648,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>45908</v>
       </c>
@@ -665,7 +665,7 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -682,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -702,7 +702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -720,7 +720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -738,7 +738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -756,7 +756,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -772,7 +772,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -780,7 +780,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>45915</v>
       </c>
@@ -797,7 +797,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
@@ -814,7 +814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -837,7 +837,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -857,7 +857,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -877,7 +877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -897,7 +897,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>45922</v>
       </c>
@@ -932,7 +932,7 @@
         <v>45926</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>0</v>
       </c>
@@ -949,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -972,7 +972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -992,7 +992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>45929</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>45933</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="F38" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>45936</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>45940</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -1312,20 +1312,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919050A3-06F3-4B9A-A699-9994F4BF1FC6}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1357,7 +1357,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>45943</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>45947</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1497,7 +1497,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>45950</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>45954</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>45957</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>45961</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>0</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>45964</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>45968</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1898,16 +1898,16 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -1917,7 +1917,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
@@ -1927,7 +1927,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1939,7 +1939,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>45964</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>45968</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>45971</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>45975</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2203,7 +2203,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>45978</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>45982</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>0</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -2289,7 +2289,7 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>45985</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>45989</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>0</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -2460,6 +2460,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b3f78198-29fa-40dc-a64e-451b3f068329">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006795F9309C3AB34BB3D82BE70F0FEC9D" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c9a1d31a48d4168ae78733f71e7b2efa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b3f78198-29fa-40dc-a64e-451b3f068329" xmlns:ns3="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e56f88943290b30cde4a9180a750d4bc" ns2:_="" ns3:_="">
     <xsd:import namespace="b3f78198-29fa-40dc-a64e-451b3f068329"/>
@@ -2660,27 +2680,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BBF6F7-45B5-4869-8DD9-1923ADFF849B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065"/>
+    <ds:schemaRef ds:uri="b3f78198-29fa-40dc-a64e-451b3f068329"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b3f78198-29fa-40dc-a64e-451b3f068329">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C20D006-F2DB-48CC-90F2-66BCA9E29FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04654532-7B9D-4FE1-AA77-A4F762484E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2697,23 +2716,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C20D006-F2DB-48CC-90F2-66BCA9E29FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BBF6F7-45B5-4869-8DD9-1923ADFF849B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065"/>
-    <ds:schemaRef ds:uri="b3f78198-29fa-40dc-a64e-451b3f068329"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>